<commit_message>
changed F_CPU to 16000000Hz
adapted timer to new F_CPU
adapted UARTs to new F_CPU
start implementation of ibus processor
created radio_controller interface
calculated values for pioneer radio
</commit_message>
<xml_diff>
--- a/Berechnungen.xlsx
+++ b/Berechnungen.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="705" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="1905" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="SPI &amp; Timer" sheetId="1" r:id="rId1"/>
+    <sheet name="Widerständen" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>F_CPU, Hz</t>
   </si>
@@ -23,6 +24,72 @@
   </si>
   <si>
     <t>SPI Freq</t>
+  </si>
+  <si>
+    <t>2k2</t>
+  </si>
+  <si>
+    <t>Wert</t>
+  </si>
+  <si>
+    <t>POT1</t>
+  </si>
+  <si>
+    <t>POT2</t>
+  </si>
+  <si>
+    <t>4k4</t>
+  </si>
+  <si>
+    <t>8k8</t>
+  </si>
+  <si>
+    <t>Berechnet</t>
+  </si>
+  <si>
+    <t>12k1</t>
+  </si>
+  <si>
+    <t>16k8</t>
+  </si>
+  <si>
+    <t>23k6</t>
+  </si>
+  <si>
+    <t>6k6</t>
+  </si>
+  <si>
+    <t>33k6</t>
+  </si>
+  <si>
+    <t>48k6</t>
+  </si>
+  <si>
+    <t>Wirklichkeit</t>
+  </si>
+  <si>
+    <t>Timer prescaler</t>
+  </si>
+  <si>
+    <t>Timer clock</t>
+  </si>
+  <si>
+    <t>Timer periode</t>
+  </si>
+  <si>
+    <t>Timer periode, ms</t>
+  </si>
+  <si>
+    <t>Gesuchte Periode, ms</t>
+  </si>
+  <si>
+    <t>Counter</t>
+  </si>
+  <si>
+    <t>bei 16 MHz = 18</t>
+  </si>
+  <si>
+    <t>bei 14,745600 = 24</t>
   </si>
 </sst>
 </file>
@@ -364,27 +431,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1">
-        <v>14745600</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>16000000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -392,16 +459,276 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
         <f>B1/B2</f>
-        <v>921600</v>
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8">
+        <f>B1/B7</f>
+        <v>15625</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9">
+        <f>1/B8</f>
+        <v>6.3999999999999997E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <f>B9*1000</f>
+        <v>6.4000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13">
+        <f>B12/B10</f>
+        <v>26.5625</v>
+      </c>
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>250</v>
+      </c>
+      <c r="C2">
+        <v>251</v>
+      </c>
+      <c r="D2">
+        <f>(((50000 * (256-B2))/256)+52)+(((50000 * (256-C2))/256)+52)</f>
+        <v>2252.4375</v>
+      </c>
+      <c r="E2">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>240</v>
+      </c>
+      <c r="C3">
+        <v>250</v>
+      </c>
+      <c r="D3">
+        <f>(((50000 * (256-B3))/256)+52)+(((50000 * (256-C3))/256)+52)</f>
+        <v>4400.875</v>
+      </c>
+      <c r="E3">
+        <v>4667</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>237</v>
+      </c>
+      <c r="C4">
+        <v>230</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D10" si="0">(((50000 * (256-B4))/256)+52)+(((50000 * (256-C4))/256)+52)</f>
+        <v>8893.0625</v>
+      </c>
+      <c r="E4">
+        <v>9200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>226</v>
+      </c>
+      <c r="C5">
+        <v>225</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>12018.0625</v>
+      </c>
+      <c r="E5">
+        <v>12370</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>214</v>
+      </c>
+      <c r="C6">
+        <v>214</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>16510.25</v>
+      </c>
+      <c r="E6">
+        <v>16910</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>196</v>
+      </c>
+      <c r="C7">
+        <v>196</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>23541.5</v>
+      </c>
+      <c r="E7">
+        <v>24000</v>
+      </c>
+      <c r="G7">
+        <f>50000/256</f>
+        <v>195.3125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>240</v>
+      </c>
+      <c r="C8">
+        <v>240</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>6354</v>
+      </c>
+      <c r="E8">
+        <v>6650</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>162</v>
+      </c>
+      <c r="C9">
+        <v>182</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>32916.5</v>
+      </c>
+      <c r="E9">
+        <v>33500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>135</v>
+      </c>
+      <c r="C10">
+        <v>135</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>47369.625</v>
+      </c>
+      <c r="E10">
+        <v>48100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
some AD5293  functions implemented
some small bugfixes
</commit_message>
<xml_diff>
--- a/Berechnungen.xlsx
+++ b/Berechnungen.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Heinrich\Documents\Atmel Studio\7.0\MFL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\heinrich\Documents\Atmel Studio\7.0\MFL\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4200" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="4800" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="SPI &amp; Timer" sheetId="1" r:id="rId1"/>
@@ -257,9 +257,6 @@
     <t>Relevant für MFL</t>
   </si>
   <si>
-    <t>Rwa:</t>
-  </si>
-  <si>
     <t>Stumm</t>
   </si>
   <si>
@@ -372,6 +369,9 @@
   </si>
   <si>
     <t>D0 = 1 (device placed in shutdown mode).</t>
+  </si>
+  <si>
+    <t>Rab:</t>
   </si>
 </sst>
 </file>
@@ -523,7 +523,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -568,6 +568,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1278,8 +1279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1479,14 +1480,14 @@
         <v>75000</v>
       </c>
       <c r="B12" s="5">
-        <v>75</v>
+        <v>2</v>
       </c>
       <c r="C12" s="5">
-        <v>75</v>
+        <v>2</v>
       </c>
       <c r="D12" s="5">
         <f>(((50000 * (256-B12))/256)+52)+(((50000 * (256-C12))/256)+52)</f>
-        <v>70807.125</v>
+        <v>99322.75</v>
       </c>
     </row>
   </sheetData>
@@ -1497,10 +1498,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1515,13 +1516,13 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>75</v>
+        <v>113</v>
       </c>
       <c r="B1" s="8">
         <v>100000</v>
       </c>
       <c r="C1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D1">
         <f>B1/1024</f>
@@ -1556,52 +1557,52 @@
         <v>2200</v>
       </c>
       <c r="C3" s="9">
-        <f t="shared" ref="C3:C11" si="0">1024-((B3/$B$1)*1024)</f>
-        <v>1001.472</v>
+        <f>(B3/$B$1)*1024</f>
+        <v>22.527999999999999</v>
       </c>
       <c r="D3" s="9">
-        <f t="shared" ref="D3:D11" si="1">ROUND(C3,0)</f>
-        <v>1001</v>
+        <f t="shared" ref="D3:D13" si="0">ROUND(C3,0)</f>
+        <v>23</v>
       </c>
       <c r="E3" s="9">
-        <f t="shared" ref="E3:E11" si="2">((1024-D3)/1024)*$B$1</f>
+        <f>(D3/1024)*$B$1</f>
         <v>2246.09375</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" s="3">
         <v>4400</v>
       </c>
       <c r="C4" s="9">
+        <f t="shared" ref="C4:C13" si="1">(B4/$B$1)*1024</f>
+        <v>45.055999999999997</v>
+      </c>
+      <c r="D4" s="9">
         <f t="shared" si="0"/>
-        <v>978.94399999999996</v>
-      </c>
-      <c r="D4" s="9">
-        <f t="shared" si="1"/>
-        <v>979</v>
+        <v>45</v>
       </c>
       <c r="E4" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="E4:E13" si="2">(D4/1024)*$B$1</f>
         <v>4394.53125</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" s="3">
         <v>6600</v>
       </c>
       <c r="C5" s="9">
+        <f t="shared" si="1"/>
+        <v>67.584000000000003</v>
+      </c>
+      <c r="D5" s="9">
         <f t="shared" si="0"/>
-        <v>956.41599999999994</v>
-      </c>
-      <c r="D5" s="9">
-        <f t="shared" si="1"/>
-        <v>956</v>
+        <v>68</v>
       </c>
       <c r="E5" s="9">
         <f t="shared" si="2"/>
@@ -1610,110 +1611,110 @@
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B6" s="3">
         <v>8800</v>
       </c>
       <c r="C6" s="9">
+        <f t="shared" si="1"/>
+        <v>90.111999999999995</v>
+      </c>
+      <c r="D6" s="9">
         <f t="shared" si="0"/>
-        <v>933.88800000000003</v>
-      </c>
-      <c r="D6" s="9">
-        <f t="shared" si="1"/>
-        <v>934</v>
+        <v>90</v>
       </c>
       <c r="E6" s="9">
         <f t="shared" si="2"/>
         <v>8789.0625</v>
       </c>
       <c r="F6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B7" s="3">
         <v>12100</v>
       </c>
       <c r="C7" s="9">
+        <f t="shared" si="1"/>
+        <v>123.904</v>
+      </c>
+      <c r="D7" s="9">
         <f t="shared" si="0"/>
-        <v>900.096</v>
-      </c>
-      <c r="D7" s="9">
-        <f t="shared" si="1"/>
-        <v>900</v>
+        <v>124</v>
       </c>
       <c r="E7" s="9">
         <f t="shared" si="2"/>
         <v>12109.375</v>
       </c>
       <c r="F7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B8" s="3">
         <v>16800</v>
       </c>
       <c r="C8" s="9">
+        <f t="shared" si="1"/>
+        <v>172.03200000000001</v>
+      </c>
+      <c r="D8" s="9">
         <f t="shared" si="0"/>
-        <v>851.96799999999996</v>
-      </c>
-      <c r="D8" s="9">
-        <f t="shared" si="1"/>
-        <v>852</v>
+        <v>172</v>
       </c>
       <c r="E8" s="9">
         <f t="shared" si="2"/>
         <v>16796.875</v>
       </c>
       <c r="F8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B9" s="3">
         <v>23600</v>
       </c>
       <c r="C9" s="9">
+        <f t="shared" si="1"/>
+        <v>241.66399999999999</v>
+      </c>
+      <c r="D9" s="9">
         <f t="shared" si="0"/>
-        <v>782.33600000000001</v>
-      </c>
-      <c r="D9" s="9">
-        <f t="shared" si="1"/>
-        <v>782</v>
+        <v>242</v>
       </c>
       <c r="E9" s="9">
         <f t="shared" si="2"/>
         <v>23632.8125</v>
       </c>
       <c r="F9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B10" s="3">
         <v>33600</v>
       </c>
       <c r="C10" s="9">
+        <f t="shared" si="1"/>
+        <v>344.06400000000002</v>
+      </c>
+      <c r="D10" s="9">
         <f t="shared" si="0"/>
-        <v>679.93599999999992</v>
-      </c>
-      <c r="D10" s="9">
-        <f t="shared" si="1"/>
-        <v>680</v>
+        <v>344</v>
       </c>
       <c r="E10" s="9">
         <f t="shared" si="2"/>
@@ -1722,22 +1723,43 @@
     </row>
     <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B11" s="3">
         <v>48600</v>
       </c>
       <c r="C11" s="9">
+        <f t="shared" si="1"/>
+        <v>497.66399999999999</v>
+      </c>
+      <c r="D11" s="9">
         <f t="shared" si="0"/>
-        <v>526.33600000000001</v>
-      </c>
-      <c r="D11" s="9">
-        <f t="shared" si="1"/>
-        <v>526</v>
+        <v>498</v>
       </c>
       <c r="E11" s="9">
         <f t="shared" si="2"/>
         <v>48632.8125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="22">
+        <v>99322</v>
+      </c>
+      <c r="C13" s="9">
+        <f t="shared" si="1"/>
+        <v>1017.05728</v>
+      </c>
+      <c r="D13" s="9">
+        <v>1020</v>
+      </c>
+      <c r="E13" s="9">
+        <f t="shared" si="2"/>
+        <v>99609.375</v>
       </c>
     </row>
   </sheetData>
@@ -1961,7 +1983,7 @@
   <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2022,20 +2044,20 @@
     </row>
     <row r="2" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C2" s="21"/>
       <c r="D2" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E2" s="20"/>
       <c r="F2" s="20"/>
       <c r="G2" s="20"/>
       <c r="H2" s="20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I2" s="20"/>
       <c r="J2" s="20"/>
@@ -2052,46 +2074,46 @@
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
       <c r="D3" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="F3" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="F3" s="14" t="s">
-        <v>100</v>
-      </c>
       <c r="G3" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H3" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="I3" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="J3" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="K3" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="K3" s="15" t="s">
+      <c r="L3" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="M3" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="M3" s="15" t="s">
+      <c r="N3" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="N3" s="15" t="s">
+      <c r="O3" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="O3" s="15" t="s">
+      <c r="P3" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="P3" s="15" t="s">
-        <v>94</v>
-      </c>
       <c r="Q3" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -2117,37 +2139,37 @@
         <v>0</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I4" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J4" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K4" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L4" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M4" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N4" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O4" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P4" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q4" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="R4" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -2173,37 +2195,37 @@
         <v>1</v>
       </c>
       <c r="H5" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="I5" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="J5" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="J5" s="17" t="s">
+      <c r="K5" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="K5" s="17" t="s">
+      <c r="L5" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="L5" s="17" t="s">
+      <c r="M5" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="M5" s="17" t="s">
+      <c r="N5" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="N5" s="17" t="s">
+      <c r="O5" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="O5" s="17" t="s">
+      <c r="P5" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="P5" s="17" t="s">
-        <v>94</v>
-      </c>
       <c r="Q5" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="R5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -2229,37 +2251,37 @@
         <v>0</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I6" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K6" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L6" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M6" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N6" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O6" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P6" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q6" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="R6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -2285,37 +2307,37 @@
         <v>0</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K7" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L7" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M7" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N7" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O7" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P7" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q7" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="R7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -2341,37 +2363,37 @@
         <v>0</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I8" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K8" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L8" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M8" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N8" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O8" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="P8" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="P8" s="17" t="s">
-        <v>94</v>
-      </c>
       <c r="Q8" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="R8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -2397,37 +2419,37 @@
         <v>1</v>
       </c>
       <c r="H9" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J9" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K9" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L9" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M9" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N9" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O9" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P9" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q9" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="R9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -2480,10 +2502,10 @@
         <v>0</v>
       </c>
       <c r="Q10" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="R10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -2508,7 +2530,7 @@
       <c r="P11" s="17"/>
       <c r="Q11" s="17"/>
       <c r="R11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -2533,7 +2555,7 @@
       <c r="P12" s="17"/>
       <c r="Q12" s="17"/>
       <c r="R12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -2822,7 +2844,7 @@
         <v>0</v>
       </c>
       <c r="R24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Migrated to new Atmel Studio version
</commit_message>
<xml_diff>
--- a/Berechnungen.xlsx
+++ b/Berechnungen.xlsx
@@ -5,22 +5,23 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\heinrich\Documents\Atmel Studio\7.0\MFL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="e:\Users\Heinrich\Documents\Atmel Studio\7.0\MFL\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4800" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="6000" windowWidth="16380" windowHeight="8190" tabRatio="644" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="SPI &amp; Timer" sheetId="1" r:id="rId1"/>
     <sheet name="Belegung" sheetId="2" r:id="rId2"/>
     <sheet name="MCP42050 Widerstände" sheetId="3" r:id="rId3"/>
-    <sheet name="AD5293 Widerstände" sheetId="4" r:id="rId4"/>
-    <sheet name="ADC" sheetId="6" r:id="rId5"/>
-    <sheet name="Botschaften" sheetId="5" r:id="rId6"/>
-    <sheet name="AD5293 MAP" sheetId="7" r:id="rId7"/>
+    <sheet name="MCP42050 Widerstände Christoph" sheetId="8" r:id="rId4"/>
+    <sheet name="AD5293 Widerstände" sheetId="4" r:id="rId5"/>
+    <sheet name="ADC" sheetId="6" r:id="rId6"/>
+    <sheet name="Botschaften" sheetId="5" r:id="rId7"/>
+    <sheet name="AD5293 MAP" sheetId="7" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="135">
   <si>
     <t>F_CPU, Hz</t>
   </si>
@@ -372,12 +373,75 @@
   </si>
   <si>
     <t>Rab:</t>
+  </si>
+  <si>
+    <t>Rab in Ohm</t>
+  </si>
+  <si>
+    <t>Bedeutung</t>
+  </si>
+  <si>
+    <t>Anzeige</t>
+  </si>
+  <si>
+    <t>Suchlauf +</t>
+  </si>
+  <si>
+    <t>Suchlauf -</t>
+  </si>
+  <si>
+    <t>BT annehmen</t>
+  </si>
+  <si>
+    <t>BT ablehnen</t>
+  </si>
+  <si>
+    <t>Rw in Ohm</t>
+  </si>
+  <si>
+    <t>Dpot1</t>
+  </si>
+  <si>
+    <t>Dpot2</t>
+  </si>
+  <si>
+    <t>Rpot2</t>
+  </si>
+  <si>
+    <t>Rpot1</t>
+  </si>
+  <si>
+    <t>Rgesamt</t>
+  </si>
+  <si>
+    <t>Tolleranz in Ohm</t>
+  </si>
+  <si>
+    <t>Innerhalb der Tolleranz?</t>
+  </si>
+  <si>
+    <t>MFL-Taste</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Pfeil hoch</t>
+  </si>
+  <si>
+    <t>Pfeil runter</t>
+  </si>
+  <si>
+    <t>R/T</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -436,7 +500,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -452,6 +516,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -523,7 +593,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -556,6 +626,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -568,7 +645,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -587,7 +663,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -851,7 +927,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1280,16 +1358,16 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.28515625" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1498,11 +1576,375 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="H5" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="I5" s="22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="21">
+        <v>1200</v>
+      </c>
+      <c r="C6">
+        <v>255</v>
+      </c>
+      <c r="D6">
+        <f>ROUND((($B$1*(256-C6))/256)+$B$2,0)</f>
+        <v>320</v>
+      </c>
+      <c r="E6">
+        <v>252</v>
+      </c>
+      <c r="F6">
+        <f>ROUND((($B$1*(256-E6))/256)+$B$2,0)</f>
+        <v>906</v>
+      </c>
+      <c r="G6" s="20">
+        <f>ROUND(D6+F6,0)</f>
+        <v>1226</v>
+      </c>
+      <c r="H6" s="18" t="str">
+        <f>IF(AND(G6&gt;=B6-$B$3,G6&lt;=B6+$B$3),"ja","nein")</f>
+        <v>ja</v>
+      </c>
+      <c r="I6" s="18"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="21">
+        <v>3500</v>
+      </c>
+      <c r="C7">
+        <v>248</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ref="D7:D14" si="0">ROUND((($B$1*(256-C7))/256)+$B$2,0)</f>
+        <v>1688</v>
+      </c>
+      <c r="E7">
+        <v>247</v>
+      </c>
+      <c r="F7">
+        <f t="shared" ref="F7:F14" si="1">ROUND((($B$1*(256-E7))/256)+$B$2,0)</f>
+        <v>1883</v>
+      </c>
+      <c r="G7" s="20">
+        <f t="shared" ref="G7:G14" si="2">ROUND(D7+F7,0)</f>
+        <v>3571</v>
+      </c>
+      <c r="H7" s="18" t="str">
+        <f t="shared" ref="H7:H14" si="3">IF(AND(G7&gt;=B7-$B$3,G7&lt;=B7+$B$3),"ja","nein")</f>
+        <v>ja</v>
+      </c>
+      <c r="I7" s="18"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="21">
+        <v>5750</v>
+      </c>
+      <c r="C8">
+        <v>240</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>3250</v>
+      </c>
+      <c r="E8">
+        <v>244</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>2469</v>
+      </c>
+      <c r="G8" s="20">
+        <f t="shared" si="2"/>
+        <v>5719</v>
+      </c>
+      <c r="H8" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>ja</v>
+      </c>
+      <c r="I8" s="18"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B9" s="21">
+        <v>8000</v>
+      </c>
+      <c r="C9">
+        <v>220</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>7156</v>
+      </c>
+      <c r="E9">
+        <v>252</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>906</v>
+      </c>
+      <c r="G9" s="20">
+        <f t="shared" si="2"/>
+        <v>8062</v>
+      </c>
+      <c r="H9" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>ja</v>
+      </c>
+      <c r="I9" s="18" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B10" s="21">
+        <v>11250</v>
+      </c>
+      <c r="C10">
+        <v>226</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>5984</v>
+      </c>
+      <c r="E10">
+        <v>230</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>5203</v>
+      </c>
+      <c r="G10" s="20">
+        <f t="shared" si="2"/>
+        <v>11187</v>
+      </c>
+      <c r="H10" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>ja</v>
+      </c>
+      <c r="I10" s="18" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="21">
+        <v>16000</v>
+      </c>
+      <c r="C11">
+        <v>215</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>8133</v>
+      </c>
+      <c r="E11">
+        <v>216</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>7938</v>
+      </c>
+      <c r="G11" s="20">
+        <f t="shared" si="2"/>
+        <v>16071</v>
+      </c>
+      <c r="H11" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>ja</v>
+      </c>
+      <c r="I11" s="18" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="21">
+        <v>24000</v>
+      </c>
+      <c r="C12">
+        <v>195</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>12039</v>
+      </c>
+      <c r="E12">
+        <v>195</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>12039</v>
+      </c>
+      <c r="G12" s="20">
+        <f t="shared" si="2"/>
+        <v>24078</v>
+      </c>
+      <c r="H12" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>ja</v>
+      </c>
+      <c r="I12" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B13" s="21">
+        <v>33000</v>
+      </c>
+      <c r="C13">
+        <v>172</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>16531</v>
+      </c>
+      <c r="E13">
+        <v>172</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>16531</v>
+      </c>
+      <c r="G13" s="20">
+        <f t="shared" si="2"/>
+        <v>33062</v>
+      </c>
+      <c r="H13" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>ja</v>
+      </c>
+      <c r="I13" s="18" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B14" s="21">
+        <v>48000</v>
+      </c>
+      <c r="C14">
+        <v>134</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>23953</v>
+      </c>
+      <c r="E14">
+        <v>134</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>23953</v>
+      </c>
+      <c r="G14" s="20">
+        <f t="shared" si="2"/>
+        <v>47906</v>
+      </c>
+      <c r="H14" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>ja</v>
+      </c>
+      <c r="I14" s="18"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="597" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1561,7 +2003,7 @@
         <v>22.527999999999999</v>
       </c>
       <c r="D3" s="9">
-        <f t="shared" ref="D3:D13" si="0">ROUND(C3,0)</f>
+        <f t="shared" ref="D3:D11" si="0">ROUND(C3,0)</f>
         <v>23</v>
       </c>
       <c r="E3" s="9">
@@ -1747,7 +2189,7 @@
       <c r="E12" s="9"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="22">
+      <c r="B13" s="19">
         <v>99322</v>
       </c>
       <c r="C13" s="9">
@@ -1768,20 +2210,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>62</v>
       </c>
@@ -1789,7 +2232,7 @@
         <v>13.2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>63</v>
       </c>
@@ -1797,7 +2240,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>64</v>
       </c>
@@ -1805,7 +2248,7 @@
         <v>4.71</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -1813,24 +2256,24 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>61</v>
       </c>
       <c r="B6">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>65</v>
       </c>
       <c r="B7">
         <f>POWER(2,B6)</f>
-        <v>256</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>67</v>
       </c>
@@ -1838,30 +2281,38 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>66</v>
       </c>
       <c r="B9">
         <f>B8/B7</f>
-        <v>1.953125E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4.8828125E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>68</v>
       </c>
       <c r="B10">
         <f>ROUND(B3/$B$9, 0)</f>
-        <v>241</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>965</v>
+      </c>
+      <c r="C10">
+        <f>B10/4</f>
+        <v>241.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>68</v>
       </c>
       <c r="B11">
         <f>ROUND(B4/$B$9, 0)</f>
+        <v>840</v>
+      </c>
+      <c r="C11">
+        <f>B11/4</f>
         <v>210</v>
       </c>
     </row>
@@ -1870,7 +2321,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -1920,11 +2371,11 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1978,7 +2429,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R24"/>
   <sheetViews>
@@ -2043,34 +2494,34 @@
       </c>
     </row>
     <row r="2" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="20" t="s">
+      <c r="C2" s="26"/>
+      <c r="D2" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20" t="s">
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="25"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
+      <c r="A3" s="24"/>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
       <c r="D3" s="14" t="s">

</xml_diff>